<commit_message>
Added DataProvider with excel
</commit_message>
<xml_diff>
--- a/test-data/orange-test-data.xlsx
+++ b/test-data/orange-test-data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>Username</t>
   </si>
@@ -30,9 +30,6 @@
     <t>Expected Error</t>
   </si>
   <si>
-    <t>Kevin</t>
-  </si>
-  <si>
     <t>Invalid credentials</t>
   </si>
   <si>
@@ -88,6 +85,12 @@
   </si>
   <si>
     <t>Time at Work</t>
+  </si>
+  <si>
+    <t>Bala</t>
+  </si>
+  <si>
+    <t>kim124</t>
   </si>
 </sst>
 </file>
@@ -386,10 +389,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
@@ -410,24 +413,35 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1">
         <v>3333</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A4" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -454,56 +468,56 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -530,18 +544,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>